<commit_message>
Fixed id for CRV, added combined excel sheet
</commit_message>
<xml_diff>
--- a/criteria1_clean_weighted.xlsx
+++ b/criteria1_clean_weighted.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29900" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="criteria1_clean_weighted" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>make</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Pricing Score</t>
+  </si>
+  <si>
+    <t>Safety Score Index</t>
   </si>
 </sst>
 </file>
@@ -247,21 +250,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>criteria1_clean_weighted!$L$2:$L$5</c:f>
+              <c:f>criteria1_clean_weighted!$M$2:$M$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.818181818181818</c:v>
+                  <c:v>0.972108014779744</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.73531774848182</c:v>
+                  <c:v>0.980602365818597</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.724552353527011</c:v>
+                  <c:v>0.973472899340407</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.71276730819956</c:v>
+                  <c:v>0.959783645266895</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -277,11 +280,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="863347280"/>
-        <c:axId val="878523984"/>
+        <c:axId val="-1586183408"/>
+        <c:axId val="-1546117680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="863347280"/>
+        <c:axId val="-1586183408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -324,7 +327,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="878523984"/>
+        <c:crossAx val="-1546117680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -332,7 +335,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="878523984"/>
+        <c:axId val="-1546117680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -382,7 +385,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="863347280"/>
+        <c:crossAx val="-1586183408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -978,16 +981,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>673100</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1010,16 +1013,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L5" totalsRowShown="0">
-  <autoFilter ref="A1:L5"/>
-  <sortState ref="A2:L5">
-    <sortCondition ref="L1:L5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:M5" totalsRowShown="0">
+  <autoFilter ref="A1:M5"/>
+  <sortState ref="A2:M5">
+    <sortCondition ref="M1:M5"/>
   </sortState>
-  <tableColumns count="12">
+  <tableColumns count="13">
     <tableColumn id="1" name="make"/>
     <tableColumn id="2" name="model"/>
     <tableColumn id="3" name="year"/>
     <tableColumn id="4" name="safety_rating"/>
+    <tableColumn id="13" name="Safety Score Index">
+      <calculatedColumnFormula>Table1[[#This Row],[safety_rating]]/MAX(Table1[safety_rating])</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="5" name="maintenance"/>
     <tableColumn id="6" name="main_cost_index" dataDxfId="1">
       <calculatedColumnFormula>MIN(Table1[maintenance])/Table1[[#This Row],[maintenance]]</calculatedColumnFormula>
@@ -1029,12 +1035,16 @@
       <calculatedColumnFormula>MIN(Table1[price_point])/Table1[[#This Row],[price_point]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" name="Safety score" dataDxfId="0">
-      <calculatedColumnFormula>Table1[[#This Row],[safety_rating]]*C7</calculatedColumnFormula>
+      <calculatedColumnFormula>Table1[[#This Row],[Safety Score Index]]*C8</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Maintainence Score"/>
-    <tableColumn id="11" name="Pricing Score"/>
+    <tableColumn id="10" name="Maintainence Score">
+      <calculatedColumnFormula>Table1[[#This Row],[main_cost_index]]*C9</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" name="Pricing Score">
+      <calculatedColumnFormula>Table1[[#This Row],[price_index]]*C10</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="12" name="Weighted score">
-      <calculatedColumnFormula>SUM(I2:K2)</calculatedColumnFormula>
+      <calculatedColumnFormula>SUM(Table1[[#This Row],[Safety score]],Table1[[#This Row],[Maintainence Score]],Table1[[#This Row],[Pricing Score]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1304,26 +1314,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCellId="1" sqref="I1:K5 A1:A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="14.5" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" customWidth="1"/>
-    <col min="9" max="9" width="13.83203125" customWidth="1"/>
-    <col min="10" max="10" width="20.1640625" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" customWidth="1"/>
+    <col min="10" max="10" width="13.83203125" customWidth="1"/>
+    <col min="11" max="11" width="20.1640625" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1337,31 +1348,34 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>23</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1375,125 +1389,137 @@
         <v>5</v>
       </c>
       <c r="E2">
-        <v>1937</v>
+        <f>Table1[[#This Row],[safety_rating]]/MAX(Table1[safety_rating])</f>
+        <v>1</v>
       </c>
       <c r="F2">
+        <v>2182</v>
+      </c>
+      <c r="G2">
+        <f>MIN(Table1[maintenance])/Table1[[#This Row],[maintenance]]</f>
+        <v>0.8982584784601283</v>
+      </c>
+      <c r="H2">
+        <v>25020</v>
+      </c>
+      <c r="I2">
+        <f>MIN(Table1[price_point])/Table1[[#This Row],[price_point]]</f>
+        <v>0.98501199040767384</v>
+      </c>
+      <c r="J2">
+        <f>Table1[[#This Row],[Safety Score Index]]*C8</f>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="K2">
+        <f>Table1[[#This Row],[main_cost_index]]*C9</f>
+        <v>0.2041496541954837</v>
+      </c>
+      <c r="L2">
+        <f>Table1[[#This Row],[price_index]]*C10</f>
+        <v>0.31341290603880528</v>
+      </c>
+      <c r="M2">
+        <f>SUM(Table1[[#This Row],[Safety score]],Table1[[#This Row],[Maintainence Score]],Table1[[#This Row],[Pricing Score]])</f>
+        <v>0.97210801477974362</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>2017</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <f>Table1[[#This Row],[safety_rating]]/MAX(Table1[safety_rating])</f>
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1960</v>
+      </c>
+      <c r="G3">
         <f>MIN(Table1[maintenance])/Table1[[#This Row],[maintenance]]</f>
         <v>1</v>
       </c>
-      <c r="G2">
-        <v>19630</v>
-      </c>
-      <c r="H2">
+      <c r="H3">
+        <v>26245</v>
+      </c>
+      <c r="I3">
+        <f>MIN(Table1[price_point])/Table1[[#This Row],[price_point]]</f>
+        <v>0.93903600685844923</v>
+      </c>
+      <c r="J3">
+        <f>Table1[[#This Row],[Safety Score Index]]*C8</f>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="K3">
+        <f>Table1[[#This Row],[main_cost_index]]*C9</f>
+        <v>0.22727272727272727</v>
+      </c>
+      <c r="L3">
+        <f>Table1[[#This Row],[price_index]]*C10</f>
+        <v>0.29878418400041568</v>
+      </c>
+      <c r="M3">
+        <f>SUM(Table1[[#This Row],[Safety score]],Table1[[#This Row],[Maintainence Score]],Table1[[#This Row],[Pricing Score]])</f>
+        <v>0.98060236581859739</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>2017</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <f>Table1[[#This Row],[safety_rating]]/MAX(Table1[safety_rating])</f>
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>2219</v>
+      </c>
+      <c r="G4">
+        <f>MIN(Table1[maintenance])/Table1[[#This Row],[maintenance]]</f>
+        <v>0.88328075709779175</v>
+      </c>
+      <c r="H4">
+        <v>24645</v>
+      </c>
+      <c r="I4">
         <f>MIN(Table1[price_point])/Table1[[#This Row],[price_point]]</f>
         <v>1</v>
       </c>
-      <c r="I2">
-        <f>Table1[[#This Row],[safety_rating]]*C8</f>
-        <v>2.2727272727272725</v>
-      </c>
-      <c r="J2">
-        <f>F2*C9</f>
-        <v>0.22727272727272727</v>
-      </c>
-      <c r="K2">
-        <f>(H2*C10)</f>
+      <c r="J4">
+        <f>Table1[[#This Row],[Safety Score Index]]*C8</f>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="K4">
+        <f>Table1[[#This Row],[main_cost_index]]*C9</f>
+        <v>0.20074562661313447</v>
+      </c>
+      <c r="L4">
+        <f>Table1[[#This Row],[price_index]]*C10</f>
         <v>0.31818181818181818</v>
       </c>
-      <c r="L2">
-        <f>SUM(I2:K2)</f>
-        <v>2.8181818181818179</v>
+      <c r="M4">
+        <f>SUM(Table1[[#This Row],[Safety score]],Table1[[#This Row],[Maintainence Score]],Table1[[#This Row],[Pricing Score]])</f>
+        <v>0.97347289934040715</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3">
-        <v>2017</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>1960</v>
-      </c>
-      <c r="F3">
-        <f>MIN(Table1[maintenance])/Table1[[#This Row],[maintenance]]</f>
-        <v>0.98826530612244901</v>
-      </c>
-      <c r="G3">
-        <v>26245</v>
-      </c>
-      <c r="H3">
-        <f>MIN(Table1[price_point])/Table1[[#This Row],[price_point]]</f>
-        <v>0.74795199085540098</v>
-      </c>
-      <c r="I3">
-        <f>Table1[[#This Row],[safety_rating]]*C8</f>
-        <v>2.2727272727272725</v>
-      </c>
-      <c r="J3">
-        <f>F3*C9</f>
-        <v>0.22460575139146569</v>
-      </c>
-      <c r="K3">
-        <f>(H3*C10)</f>
-        <v>0.23798472436308213</v>
-      </c>
-      <c r="L3">
-        <f>SUM(I3:K3)</f>
-        <v>2.7353177484818203</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>2017</v>
-      </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
-      <c r="E4">
-        <v>2219</v>
-      </c>
-      <c r="F4">
-        <f>MIN(Table1[maintenance])/Table1[[#This Row],[maintenance]]</f>
-        <v>0.87291572780531768</v>
-      </c>
-      <c r="G4">
-        <v>24645</v>
-      </c>
-      <c r="H4">
-        <f>MIN(Table1[price_point])/Table1[[#This Row],[price_point]]</f>
-        <v>0.79651044836680873</v>
-      </c>
-      <c r="I4">
-        <f>Table1[[#This Row],[safety_rating]]*C8</f>
-        <v>2.2727272727272725</v>
-      </c>
-      <c r="J4">
-        <f>F4*C9</f>
-        <v>0.19838993813757219</v>
-      </c>
-      <c r="K4">
-        <f>(H4*C10)</f>
-        <v>0.25343514266216643</v>
-      </c>
-      <c r="L4">
-        <f>SUM(I4:K4)</f>
-        <v>2.7245523535270113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1507,37 +1533,41 @@
         <v>5</v>
       </c>
       <c r="E5">
+        <f>Table1[[#This Row],[safety_rating]]/MAX(Table1[safety_rating])</f>
+        <v>1</v>
+      </c>
+      <c r="F5">
         <v>2271</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <f>MIN(Table1[maintenance])/Table1[[#This Row],[maintenance]]</f>
-        <v>0.85292822545134306</v>
-      </c>
-      <c r="G5">
+        <v>0.86305592250110086</v>
+      </c>
+      <c r="H5">
         <v>25370</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <f>MIN(Table1[price_point])/Table1[[#This Row],[price_point]]</f>
-        <v>0.77374852187623178</v>
-      </c>
-      <c r="I5">
-        <f>Table1[[#This Row],[safety_rating]]*C8</f>
-        <v>2.2727272727272725</v>
+        <v>0.97142294048088296</v>
       </c>
       <c r="J5">
-        <f>F5*C9</f>
-        <v>0.19384732396621432</v>
+        <f>Table1[[#This Row],[Safety Score Index]]*C8</f>
+        <v>0.45454545454545453</v>
       </c>
       <c r="K5">
-        <f>(H5*C10)</f>
-        <v>0.24619271150607375</v>
+        <f>Table1[[#This Row],[main_cost_index]]*C9</f>
+        <v>0.19614907329570475</v>
       </c>
       <c r="L5">
-        <f>SUM(I5:K5)</f>
-        <v>2.7127673081995605</v>
+        <f>Table1[[#This Row],[price_index]]*C10</f>
+        <v>0.30908911742573547</v>
+      </c>
+      <c r="M5">
+        <f>SUM(Table1[[#This Row],[Safety score]],Table1[[#This Row],[Maintainence Score]],Table1[[#This Row],[Pricing Score]])</f>
+        <v>0.95978364526689486</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>19</v>
       </c>
@@ -1545,7 +1575,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1557,7 +1587,7 @@
         <v>0.45454545454545453</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1569,7 +1599,7 @@
         <v>0.22727272727272727</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>

</xml_diff>